<commit_message>
Fix farm_crop and farm_field crash
</commit_message>
<xml_diff>
--- a/app/config/tables/farm_crop/forms/farm_crop/farm_crop.xlsx
+++ b/app/config/tables/farm_crop/forms/farm_crop/farm_crop.xlsx
@@ -4,15 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="10620" yWindow="0" windowWidth="30300" windowHeight="20300" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
     <sheet name="survey" sheetId="1" r:id="rId2"/>
-    <sheet name="properties" sheetId="6" r:id="rId3"/>
-    <sheet name="model" sheetId="7" r:id="rId4"/>
-    <sheet name="settings" sheetId="3" r:id="rId5"/>
-    <sheet name="queries" sheetId="8" r:id="rId6"/>
+    <sheet name="model" sheetId="7" r:id="rId3"/>
+    <sheet name="settings" sheetId="3" r:id="rId4"/>
+    <sheet name="queries" sheetId="8" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
   <si>
     <t>clause</t>
   </si>
@@ -126,27 +125,6 @@
   </si>
   <si>
     <t>Crops</t>
-  </si>
-  <si>
-    <t>partition</t>
-  </si>
-  <si>
-    <t>aspect</t>
-  </si>
-  <si>
-    <t>key</t>
-  </si>
-  <si>
-    <t>Table</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>colOrder</t>
-  </si>
-  <si>
-    <t>object</t>
   </si>
   <si>
     <t>instance_name</t>
@@ -217,9 +195,6 @@
   </si>
   <si>
     <t>select_one_dropdown</t>
-  </si>
-  <si>
-    <t>["farm_name","farm_uuid","location_latitude","location_longitude","location_altitude","location_accuracy","farm_num_employee","farm_revenue","field_name","field_uuid","crop_name","num_crop","crop_pesticides","crop_fertilizer","crop_harvest"]</t>
   </si>
   <si>
     <t>farm_uuid</t>
@@ -811,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -849,7 +824,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="60">
@@ -861,7 +836,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="4"/>
       <c r="F2" s="9" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -956,65 +931,176 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="E10" s="4"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="E14" s="4"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="F16" s="1"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="30" spans="6:8">
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="6:8">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="6:8">
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="6:8">
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1029,176 +1115,70 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="4" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20160210</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="30" spans="6:8">
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="6:8">
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="6:8">
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="6:8">
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1212,81 +1192,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:3" ht="30">
-      <c r="A1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="1">
-        <v>20160210</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -1304,44 +1209,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="45">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4">

</xml_diff>

<commit_message>
Fixes to generate proper choice list from csv and ajax queries (need to change from display.text to display.title.text )
</commit_message>
<xml_diff>
--- a/app/config/tables/farm_crop/forms/farm_crop/farm_crop.xlsx
+++ b/app/config/tables/farm_crop/forms/farm_crop/farm_crop.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10617" yWindow="0" windowWidth="30305" windowHeight="20304" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="10617" yWindow="0" windowWidth="30305" windowHeight="20304" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -156,59 +156,59 @@
     <t>pesticides_csv</t>
   </si>
   <si>
+    <t>select_multiple_inline</t>
+  </si>
+  <si>
+    <t>fertilizer_csv</t>
+  </si>
+  <si>
+    <t>"fertilizer.csv"</t>
+  </si>
+  <si>
+    <t>"pesticides.csv"</t>
+  </si>
+  <si>
+    <t>field_name</t>
+  </si>
+  <si>
+    <t>farm_state</t>
+  </si>
+  <si>
+    <t>farm_city</t>
+  </si>
+  <si>
+    <t>select_one_dropdown</t>
+  </si>
+  <si>
+    <t>farm_uuid</t>
+  </si>
+  <si>
+    <t>field_uuid</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>Data for field: {{data.field_uuid}}</t>
+  </si>
+  <si>
+    <t>display.title.text</t>
+  </si>
+  <si>
+    <t>display.prompt.text</t>
+  </si>
+  <si>
+    <t>display.hint.text</t>
+  </si>
+  <si>
     <t>_.chain(context).pluck('pesticides').uniq().map(function(pesticides){
-return {name:pesticides, label:pesticides, data_value:pesticides, display:{text:pesticides}};
+return { data_value:pesticides, display: {title: {text:pesticides} } };
 }).value()</t>
   </si>
   <si>
-    <t>select_multiple_inline</t>
-  </si>
-  <si>
-    <t>fertilizer_csv</t>
-  </si>
-  <si>
-    <t>"fertilizer.csv"</t>
-  </si>
-  <si>
     <t>_.chain(context).pluck('fertilizer').uniq().map(function(fertilizer){
-return {name:fertilizer, label:fertilizer, data_value:fertilizer, display:{text:fertilizer}};
+return { data_value:fertilizer, display:{title: {text: fertilizer} } };
 }).value()</t>
-  </si>
-  <si>
-    <t>"pesticides.csv"</t>
-  </si>
-  <si>
-    <t>field_name</t>
-  </si>
-  <si>
-    <t>farm_state</t>
-  </si>
-  <si>
-    <t>farm_city</t>
-  </si>
-  <si>
-    <t>select_one_dropdown</t>
-  </si>
-  <si>
-    <t>farm_uuid</t>
-  </si>
-  <si>
-    <t>field_uuid</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>Data for field: {{data.field_uuid}}</t>
-  </si>
-  <si>
-    <t>display.title.text</t>
-  </si>
-  <si>
-    <t>display.prompt.text</t>
-  </si>
-  <si>
-    <t>display.hint.text</t>
   </si>
 </sst>
 </file>
@@ -757,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>26</v>
@@ -807,7 +807,7 @@
     <col min="8" max="8" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -824,16 +824,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="31.45" x14ac:dyDescent="0.3">
@@ -845,7 +845,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="4"/>
       <c r="F2" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -963,7 +963,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -971,18 +971,18 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1011,7 +1011,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
@@ -1052,7 +1052,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1063,7 +1063,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1120,7 +1120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1138,7 +1138,7 @@
         <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1199,8 +1199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1233,24 +1233,24 @@
         <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="47.15" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>